<commit_message>
sin apocalypse english name
</commit_message>
<xml_diff>
--- a/sin-apocalypse/checklist.xlsx
+++ b/sin-apocalypse/checklist.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/sin-apocalypse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C6C723D-6894-DC4D-A1CE-68AEA49D7678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{682F3B19-463B-9842-AB93-FA6B6DDEA431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{DE3CA47A-EF56-8043-842B-F92F02DA4BA9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="checklist" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -63,10 +63,10 @@
     <t xml:space="preserve">新世黙示録 </t>
   </si>
   <si>
-    <t>New World Apocalypse</t>
-  </si>
-  <si>
     <t>Enterbrain</t>
+  </si>
+  <si>
+    <t>Sin Apocalypse</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,10 +468,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>

</xml_diff>